<commit_message>
Updates with 2020 data
Cleans up 2019 data a bit with additional code and then adds in the new 2020 Census data relating to the ACS for population and housing estimates by interested zip codes. Relabels files to reflect both years
</commit_message>
<xml_diff>
--- a/2019ACS_DemographicHousingEstimates_WorkingCopy.xlsx
+++ b/2019ACS_DemographicHousingEstimates_WorkingCopy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://floridahealth-my.sharepoint.com/personal/michelle_slawinski_flhealth_gov/Documents/Documents/Projects/Resource Map/Data/Demographic &amp; Housing Estimates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://floridahealth-my.sharepoint.com/personal/michelle_slawinski_flhealth_gov/Documents/Documents/GitHub/Census/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="440" documentId="8_{6EF9E7D6-0E32-4527-82C6-5D74BBD9F8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17FBC63E-EBB3-4654-99BA-C61694958510}"/>
+  <xr:revisionPtr revIDLastSave="448" documentId="8_{6EF9E7D6-0E32-4527-82C6-5D74BBD9F8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6ED64771-055C-4156-929A-215C40B482F3}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F5BEBB51-587C-4DC1-8147-8A3F0C77C96A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F5BEBB51-587C-4DC1-8147-8A3F0C77C96A}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Discard" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Dictionary!$A$1:$C$165</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Dictionary!$A$1:$C$163</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3350,17 +3350,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E68C49-8AE4-40E1-B1F5-2DFF9F435EA4}">
   <dimension ref="A1:MT57"/>
   <sheetViews>
-    <sheetView topLeftCell="BR1" workbookViewId="0">
-      <selection activeCell="CC3" activeCellId="2" sqref="CE3 CC2 CC3"/>
+    <sheetView topLeftCell="LS1" workbookViewId="0">
+      <selection activeCell="MH21" sqref="MH21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="70" max="70" width="63.28515625" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="46.140625" customWidth="1"/>
     <col min="82" max="82" width="19.140625" customWidth="1"/>
     <col min="83" max="83" width="21.140625" customWidth="1"/>
     <col min="84" max="84" width="18.85546875" customWidth="1"/>
     <col min="97" max="97" width="26.28515625" customWidth="1"/>
+    <col min="356" max="356" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:358" x14ac:dyDescent="0.25">
@@ -64702,10 +64704,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E594E6-292A-489C-8899-DB3004E2AD40}">
-  <dimension ref="A1:D165"/>
+  <dimension ref="A1:D163"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A162" sqref="A162"/>
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -66434,107 +66436,89 @@
         <v>961</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>684</v>
-      </c>
-      <c r="C157" t="s">
-        <v>964</v>
+        <v>686</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>965</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>694</v>
+        <v>698</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>356</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>698</v>
-      </c>
-      <c r="C164" s="4" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>357</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>699</v>
-      </c>
-      <c r="C165" s="4" t="s">
         <v>972</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C165" xr:uid="{63E594E6-292A-489C-8899-DB3004E2AD40}"/>
+  <autoFilter ref="A1:C163" xr:uid="{63E594E6-292A-489C-8899-DB3004E2AD40}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C163">
+      <sortCondition ref="A1:A163"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -66542,10 +66526,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD051FDE-368E-43E7-93C7-ED9FE59F8A2D}">
-  <dimension ref="A1:D195"/>
+  <dimension ref="A1:D197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="B181" sqref="B181"/>
+    <sheetView topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="C180" sqref="C180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -68214,6 +68198,28 @@
         <v>976</v>
       </c>
     </row>
+    <row r="196" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="B196" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="C196" s="4" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A197" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="B197" s="5" t="s">
+        <v>688</v>
+      </c>
+      <c r="C197" s="4" t="s">
+        <v>966</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>